<commit_message>
dataset Us Crime agregado
</commit_message>
<xml_diff>
--- a/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/log_pcsmote_x_muestra_ecoli_D25_R25_PPproporcion.xlsx
+++ b/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/log_pcsmote_x_muestra_ecoli_D25_R25_PPproporcion.xlsx
@@ -657,7 +657,7 @@
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.045715</t>
+          <t>2025-11-13T06:53:19.255633</t>
         </is>
       </c>
     </row>
@@ -747,7 +747,7 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.045715</t>
+          <t>2025-11-13T06:53:19.256633</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.046720</t>
+          <t>2025-11-13T06:53:19.256633</t>
         </is>
       </c>
     </row>
@@ -927,7 +927,7 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.046720</t>
+          <t>2025-11-13T06:53:19.256633</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.047716</t>
+          <t>2025-11-13T06:53:19.256633</t>
         </is>
       </c>
     </row>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.047716</t>
+          <t>2025-11-13T06:53:19.256633</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.048713</t>
+          <t>2025-11-13T06:53:19.256633</t>
         </is>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.048713</t>
+          <t>2025-11-13T06:53:19.256633</t>
         </is>
       </c>
     </row>
@@ -1373,7 +1373,7 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.049717</t>
+          <t>2025-11-13T06:53:19.256633</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.049717</t>
+          <t>2025-11-13T06:53:19.256633</t>
         </is>
       </c>
     </row>
@@ -1549,7 +1549,7 @@
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.049717</t>
+          <t>2025-11-13T06:53:19.256633</t>
         </is>
       </c>
     </row>
@@ -1635,7 +1635,7 @@
       <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.050717</t>
+          <t>2025-11-13T06:53:19.257633</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.050717</t>
+          <t>2025-11-13T06:53:19.257633</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.051717</t>
+          <t>2025-11-13T06:53:19.257633</t>
         </is>
       </c>
     </row>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.052162</t>
+          <t>2025-11-13T06:53:19.257633</t>
         </is>
       </c>
     </row>
@@ -1995,7 +1995,7 @@
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.052717</t>
+          <t>2025-11-13T06:53:19.257633</t>
         </is>
       </c>
     </row>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.052717</t>
+          <t>2025-11-13T06:53:19.257633</t>
         </is>
       </c>
     </row>
@@ -2171,7 +2171,7 @@
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.052717</t>
+          <t>2025-11-13T06:53:19.257633</t>
         </is>
       </c>
     </row>
@@ -2257,7 +2257,7 @@
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.053977</t>
+          <t>2025-11-13T06:53:19.257633</t>
         </is>
       </c>
     </row>
@@ -2347,7 +2347,7 @@
       </c>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.053977</t>
+          <t>2025-11-13T06:53:19.257633</t>
         </is>
       </c>
     </row>
@@ -2437,7 +2437,7 @@
       </c>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.057512</t>
+          <t>2025-11-13T06:53:19.257633</t>
         </is>
       </c>
     </row>
@@ -2523,7 +2523,7 @@
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.057512</t>
+          <t>2025-11-13T06:53:19.258633</t>
         </is>
       </c>
     </row>
@@ -2613,7 +2613,7 @@
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.058517</t>
+          <t>2025-11-13T06:53:19.258633</t>
         </is>
       </c>
     </row>
@@ -2703,7 +2703,7 @@
       </c>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.059510</t>
+          <t>2025-11-13T06:53:19.258633</t>
         </is>
       </c>
     </row>
@@ -2789,7 +2789,7 @@
       <c r="Y26" t="inlineStr"/>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.059510</t>
+          <t>2025-11-13T06:53:19.258633</t>
         </is>
       </c>
     </row>
@@ -2875,7 +2875,7 @@
       <c r="Y27" t="inlineStr"/>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.060506</t>
+          <t>2025-11-13T06:53:19.258633</t>
         </is>
       </c>
     </row>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.060506</t>
+          <t>2025-11-13T06:53:19.258633</t>
         </is>
       </c>
     </row>
@@ -3055,7 +3055,7 @@
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.061507</t>
+          <t>2025-11-13T06:53:19.258633</t>
         </is>
       </c>
     </row>
@@ -3145,7 +3145,7 @@
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.061507</t>
+          <t>2025-11-13T06:53:19.258633</t>
         </is>
       </c>
     </row>
@@ -3231,7 +3231,7 @@
       <c r="Y31" t="inlineStr"/>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.061507</t>
+          <t>2025-11-13T06:53:19.258633</t>
         </is>
       </c>
     </row>
@@ -3317,7 +3317,7 @@
       <c r="Y32" t="inlineStr"/>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.062510</t>
+          <t>2025-11-13T06:53:19.258633</t>
         </is>
       </c>
     </row>
@@ -3403,7 +3403,7 @@
       <c r="Y33" t="inlineStr"/>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.062510</t>
+          <t>2025-11-13T06:53:19.258633</t>
         </is>
       </c>
     </row>
@@ -3493,7 +3493,7 @@
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.062510</t>
+          <t>2025-11-13T06:53:19.259633</t>
         </is>
       </c>
     </row>
@@ -3583,7 +3583,7 @@
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.063509</t>
+          <t>2025-11-13T06:53:19.259633</t>
         </is>
       </c>
     </row>
@@ -3673,7 +3673,7 @@
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.063509</t>
+          <t>2025-11-13T06:53:19.259633</t>
         </is>
       </c>
     </row>
@@ -3759,7 +3759,7 @@
       <c r="Y37" t="inlineStr"/>
       <c r="Z37" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.064506</t>
+          <t>2025-11-13T06:53:19.259633</t>
         </is>
       </c>
     </row>
@@ -3845,7 +3845,7 @@
       <c r="Y38" t="inlineStr"/>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.065504</t>
+          <t>2025-11-13T06:53:19.259633</t>
         </is>
       </c>
     </row>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.065504</t>
+          <t>2025-11-13T06:53:19.259633</t>
         </is>
       </c>
     </row>
@@ -4021,7 +4021,7 @@
       <c r="Y40" t="inlineStr"/>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.066506</t>
+          <t>2025-11-13T06:53:19.259633</t>
         </is>
       </c>
     </row>
@@ -4111,7 +4111,7 @@
       </c>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.066506</t>
+          <t>2025-11-13T06:53:19.259633</t>
         </is>
       </c>
     </row>
@@ -4201,7 +4201,7 @@
       </c>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.066506</t>
+          <t>2025-11-13T06:53:19.259633</t>
         </is>
       </c>
     </row>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.259633</t>
         </is>
       </c>
     </row>
@@ -4377,7 +4377,7 @@
       <c r="Y44" t="inlineStr"/>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.259633</t>
         </is>
       </c>
     </row>
@@ -4463,7 +4463,7 @@
       <c r="Y45" t="inlineStr"/>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.260632</t>
         </is>
       </c>
     </row>
@@ -4549,7 +4549,7 @@
       <c r="Y46" t="inlineStr"/>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.260632</t>
         </is>
       </c>
     </row>
@@ -4635,7 +4635,7 @@
       <c r="Y47" t="inlineStr"/>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.260632</t>
         </is>
       </c>
     </row>
@@ -4725,7 +4725,7 @@
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.260632</t>
         </is>
       </c>
     </row>
@@ -4815,7 +4815,7 @@
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.260632</t>
         </is>
       </c>
     </row>
@@ -4901,7 +4901,7 @@
       <c r="Y50" t="inlineStr"/>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.260632</t>
         </is>
       </c>
     </row>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.260632</t>
         </is>
       </c>
     </row>
@@ -5077,7 +5077,7 @@
       <c r="Y52" t="inlineStr"/>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.260632</t>
         </is>
       </c>
     </row>
@@ -5163,7 +5163,7 @@
       <c r="Y53" t="inlineStr"/>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.260632</t>
         </is>
       </c>
     </row>
@@ -5253,7 +5253,7 @@
       </c>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.260632</t>
         </is>
       </c>
     </row>
@@ -5343,7 +5343,7 @@
       </c>
       <c r="Z55" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.261632</t>
         </is>
       </c>
     </row>
@@ -5429,7 +5429,7 @@
       <c r="Y56" t="inlineStr"/>
       <c r="Z56" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.261632</t>
         </is>
       </c>
     </row>
@@ -5519,7 +5519,7 @@
       </c>
       <c r="Z57" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.261632</t>
         </is>
       </c>
     </row>
@@ -5609,7 +5609,7 @@
       </c>
       <c r="Z58" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.261632</t>
         </is>
       </c>
     </row>
@@ -5695,7 +5695,7 @@
       <c r="Y59" t="inlineStr"/>
       <c r="Z59" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.261632</t>
         </is>
       </c>
     </row>
@@ -5785,7 +5785,7 @@
       </c>
       <c r="Z60" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.261632</t>
         </is>
       </c>
     </row>
@@ -5875,7 +5875,7 @@
       </c>
       <c r="Z61" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.261632</t>
         </is>
       </c>
     </row>
@@ -5961,7 +5961,7 @@
       <c r="Y62" t="inlineStr"/>
       <c r="Z62" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:14.073614</t>
+          <t>2025-11-13T06:53:19.261632</t>
         </is>
       </c>
     </row>
@@ -6051,7 +6051,7 @@
       </c>
       <c r="Z63" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.010417</t>
+          <t>2025-11-13T06:53:19.451899</t>
         </is>
       </c>
     </row>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="Z64" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.010417</t>
+          <t>2025-11-13T06:53:19.452899</t>
         </is>
       </c>
     </row>
@@ -6227,7 +6227,7 @@
       <c r="Y65" t="inlineStr"/>
       <c r="Z65" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.010417</t>
+          <t>2025-11-13T06:53:19.452899</t>
         </is>
       </c>
     </row>
@@ -6313,7 +6313,7 @@
       <c r="Y66" t="inlineStr"/>
       <c r="Z66" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.011409</t>
+          <t>2025-11-13T06:53:19.452899</t>
         </is>
       </c>
     </row>
@@ -6403,7 +6403,7 @@
       </c>
       <c r="Z67" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.012407</t>
+          <t>2025-11-13T06:53:19.452899</t>
         </is>
       </c>
     </row>
@@ -6493,7 +6493,7 @@
       </c>
       <c r="Z68" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.012407</t>
+          <t>2025-11-13T06:53:19.452899</t>
         </is>
       </c>
     </row>
@@ -6583,7 +6583,7 @@
       </c>
       <c r="Z69" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.013407</t>
+          <t>2025-11-13T06:53:19.452899</t>
         </is>
       </c>
     </row>
@@ -6673,7 +6673,7 @@
       </c>
       <c r="Z70" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.013407</t>
+          <t>2025-11-13T06:53:19.453900</t>
         </is>
       </c>
     </row>
@@ -6763,7 +6763,7 @@
       </c>
       <c r="Z71" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.013407</t>
+          <t>2025-11-13T06:53:19.453900</t>
         </is>
       </c>
     </row>
@@ -6853,7 +6853,7 @@
       </c>
       <c r="Z72" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.014408</t>
+          <t>2025-11-13T06:53:19.453900</t>
         </is>
       </c>
     </row>
@@ -6943,7 +6943,7 @@
       </c>
       <c r="Z73" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.014408</t>
+          <t>2025-11-13T06:53:19.453900</t>
         </is>
       </c>
     </row>
@@ -7033,7 +7033,7 @@
       </c>
       <c r="Z74" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.015406</t>
+          <t>2025-11-13T06:53:19.453900</t>
         </is>
       </c>
     </row>
@@ -7123,7 +7123,7 @@
       </c>
       <c r="Z75" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.015406</t>
+          <t>2025-11-13T06:53:19.454901</t>
         </is>
       </c>
     </row>
@@ -7213,7 +7213,7 @@
       </c>
       <c r="Z76" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.015406</t>
+          <t>2025-11-13T06:53:19.454901</t>
         </is>
       </c>
     </row>
@@ -7303,7 +7303,7 @@
       </c>
       <c r="Z77" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.016406</t>
+          <t>2025-11-13T06:53:19.454901</t>
         </is>
       </c>
     </row>
@@ -7393,7 +7393,7 @@
       </c>
       <c r="Z78" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.016406</t>
+          <t>2025-11-13T06:53:19.454901</t>
         </is>
       </c>
     </row>
@@ -7483,7 +7483,7 @@
       </c>
       <c r="Z79" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.016406</t>
+          <t>2025-11-13T06:53:19.454901</t>
         </is>
       </c>
     </row>
@@ -7573,7 +7573,7 @@
       </c>
       <c r="Z80" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.017406</t>
+          <t>2025-11-13T06:53:19.458102</t>
         </is>
       </c>
     </row>
@@ -7663,7 +7663,7 @@
       </c>
       <c r="Z81" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.017406</t>
+          <t>2025-11-13T06:53:19.458102</t>
         </is>
       </c>
     </row>
@@ -7753,7 +7753,7 @@
       </c>
       <c r="Z82" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.017406</t>
+          <t>2025-11-13T06:53:19.460551</t>
         </is>
       </c>
     </row>
@@ -7843,7 +7843,7 @@
       </c>
       <c r="Z83" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.018405</t>
+          <t>2025-11-13T06:53:19.461085</t>
         </is>
       </c>
     </row>
@@ -7933,7 +7933,7 @@
       </c>
       <c r="Z84" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.019407</t>
+          <t>2025-11-13T06:53:19.465083</t>
         </is>
       </c>
     </row>
@@ -8019,7 +8019,7 @@
       <c r="Y85" t="inlineStr"/>
       <c r="Z85" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.020407</t>
+          <t>2025-11-13T06:53:19.465083</t>
         </is>
       </c>
     </row>
@@ -8109,7 +8109,7 @@
       </c>
       <c r="Z86" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.022404</t>
+          <t>2025-11-13T06:53:19.465083</t>
         </is>
       </c>
     </row>
@@ -8195,7 +8195,7 @@
       <c r="Y87" t="inlineStr"/>
       <c r="Z87" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.022404</t>
+          <t>2025-11-13T06:53:19.465083</t>
         </is>
       </c>
     </row>
@@ -8285,7 +8285,7 @@
       </c>
       <c r="Z88" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.023407</t>
+          <t>2025-11-13T06:53:19.466085</t>
         </is>
       </c>
     </row>
@@ -8375,7 +8375,7 @@
       </c>
       <c r="Z89" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.023407</t>
+          <t>2025-11-13T06:53:19.467082</t>
         </is>
       </c>
     </row>
@@ -8465,7 +8465,7 @@
       </c>
       <c r="Z90" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.024405</t>
+          <t>2025-11-13T06:53:19.467082</t>
         </is>
       </c>
     </row>
@@ -8551,7 +8551,7 @@
       <c r="Y91" t="inlineStr"/>
       <c r="Z91" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.499280</t>
+          <t>2025-11-13T06:53:19.690274</t>
         </is>
       </c>
     </row>
@@ -8637,7 +8637,7 @@
       <c r="Y92" t="inlineStr"/>
       <c r="Z92" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.500282</t>
+          <t>2025-11-13T06:53:19.691275</t>
         </is>
       </c>
     </row>
@@ -8727,7 +8727,7 @@
       </c>
       <c r="Z93" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.500282</t>
+          <t>2025-11-13T06:53:19.691275</t>
         </is>
       </c>
     </row>
@@ -8813,7 +8813,7 @@
       <c r="Y94" t="inlineStr"/>
       <c r="Z94" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.501282</t>
+          <t>2025-11-13T06:53:19.691275</t>
         </is>
       </c>
     </row>
@@ -8899,7 +8899,7 @@
       <c r="Y95" t="inlineStr"/>
       <c r="Z95" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.501282</t>
+          <t>2025-11-13T06:53:19.692161</t>
         </is>
       </c>
     </row>
@@ -8989,7 +8989,7 @@
       </c>
       <c r="Z96" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.501282</t>
+          <t>2025-11-13T06:53:19.692161</t>
         </is>
       </c>
     </row>
@@ -9079,7 +9079,7 @@
       </c>
       <c r="Z97" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.502280</t>
+          <t>2025-11-13T06:53:19.692673</t>
         </is>
       </c>
     </row>
@@ -9165,7 +9165,7 @@
       <c r="Y98" t="inlineStr"/>
       <c r="Z98" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.502280</t>
+          <t>2025-11-13T06:53:19.692754</t>
         </is>
       </c>
     </row>
@@ -9255,7 +9255,7 @@
       </c>
       <c r="Z99" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.503280</t>
+          <t>2025-11-13T06:53:19.692754</t>
         </is>
       </c>
     </row>
@@ -9345,7 +9345,7 @@
       </c>
       <c r="Z100" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.506284</t>
+          <t>2025-11-13T06:53:19.692754</t>
         </is>
       </c>
     </row>
@@ -9435,7 +9435,7 @@
       </c>
       <c r="Z101" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.506284</t>
+          <t>2025-11-13T06:53:19.693285</t>
         </is>
       </c>
     </row>
@@ -9525,7 +9525,7 @@
       </c>
       <c r="Z102" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.507283</t>
+          <t>2025-11-13T06:53:19.693285</t>
         </is>
       </c>
     </row>
@@ -9611,7 +9611,7 @@
       <c r="Y103" t="inlineStr"/>
       <c r="Z103" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.507283</t>
+          <t>2025-11-13T06:53:19.693285</t>
         </is>
       </c>
     </row>
@@ -9701,7 +9701,7 @@
       </c>
       <c r="Z104" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.507283</t>
+          <t>2025-11-13T06:53:19.693285</t>
         </is>
       </c>
     </row>
@@ -9791,7 +9791,7 @@
       </c>
       <c r="Z105" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.508283</t>
+          <t>2025-11-13T06:53:19.693285</t>
         </is>
       </c>
     </row>
@@ -9877,7 +9877,7 @@
       <c r="Y106" t="inlineStr"/>
       <c r="Z106" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:15.509280</t>
+          <t>2025-11-13T06:53:19.693285</t>
         </is>
       </c>
     </row>
@@ -9963,7 +9963,7 @@
       <c r="Y107" t="inlineStr"/>
       <c r="Z107" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.498698</t>
+          <t>2025-11-13T06:53:19.911685</t>
         </is>
       </c>
     </row>
@@ -10053,7 +10053,7 @@
       </c>
       <c r="Z108" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.498698</t>
+          <t>2025-11-13T06:53:19.911685</t>
         </is>
       </c>
     </row>
@@ -10143,7 +10143,7 @@
       </c>
       <c r="Z109" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.499701</t>
+          <t>2025-11-13T06:53:19.911685</t>
         </is>
       </c>
     </row>
@@ -10233,7 +10233,7 @@
       </c>
       <c r="Z110" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.499701</t>
+          <t>2025-11-13T06:53:19.911685</t>
         </is>
       </c>
     </row>
@@ -10319,7 +10319,7 @@
       <c r="Y111" t="inlineStr"/>
       <c r="Z111" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.500700</t>
+          <t>2025-11-13T06:53:19.911685</t>
         </is>
       </c>
     </row>
@@ -10409,7 +10409,7 @@
       </c>
       <c r="Z112" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.500700</t>
+          <t>2025-11-13T06:53:19.912468</t>
         </is>
       </c>
     </row>
@@ -10495,7 +10495,7 @@
       <c r="Y113" t="inlineStr"/>
       <c r="Z113" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.501703</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -10581,7 +10581,7 @@
       <c r="Y114" t="inlineStr"/>
       <c r="Z114" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.501703</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -10667,7 +10667,7 @@
       <c r="Y115" t="inlineStr"/>
       <c r="Z115" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.502702</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -10757,7 +10757,7 @@
       </c>
       <c r="Z116" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.507701</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -10847,7 +10847,7 @@
       </c>
       <c r="Z117" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.507701</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -10937,7 +10937,7 @@
       </c>
       <c r="Z118" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.508700</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -11027,7 +11027,7 @@
       </c>
       <c r="Z119" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.508700</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -11113,7 +11113,7 @@
       <c r="Y120" t="inlineStr"/>
       <c r="Z120" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.509700</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -11199,7 +11199,7 @@
       <c r="Y121" t="inlineStr"/>
       <c r="Z121" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.509700</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -11285,7 +11285,7 @@
       <c r="Y122" t="inlineStr"/>
       <c r="Z122" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.509700</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -11375,7 +11375,7 @@
       </c>
       <c r="Z123" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.510700</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -11465,7 +11465,7 @@
       </c>
       <c r="Z124" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.510700</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -11551,7 +11551,7 @@
       <c r="Y125" t="inlineStr"/>
       <c r="Z125" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.511697</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -11641,7 +11641,7 @@
       </c>
       <c r="Z126" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.511697</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -11731,7 +11731,7 @@
       </c>
       <c r="Z127" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.512698</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -11821,7 +11821,7 @@
       </c>
       <c r="Z128" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.512698</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -11907,7 +11907,7 @@
       <c r="Y129" t="inlineStr"/>
       <c r="Z129" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.513701</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -11997,7 +11997,7 @@
       </c>
       <c r="Z130" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.514701</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -12087,7 +12087,7 @@
       </c>
       <c r="Z131" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.514701</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -12173,7 +12173,7 @@
       <c r="Y132" t="inlineStr"/>
       <c r="Z132" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.514701</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -12263,7 +12263,7 @@
       </c>
       <c r="Z133" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.515701</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -12353,7 +12353,7 @@
       </c>
       <c r="Z134" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.515701</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -12439,7 +12439,7 @@
       <c r="Y135" t="inlineStr"/>
       <c r="Z135" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.516701</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -12529,7 +12529,7 @@
       </c>
       <c r="Z136" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.517701</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -12615,7 +12615,7 @@
       <c r="Y137" t="inlineStr"/>
       <c r="Z137" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.517701</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -12701,7 +12701,7 @@
       <c r="Y138" t="inlineStr"/>
       <c r="Z138" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.518700</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -12791,7 +12791,7 @@
       </c>
       <c r="Z139" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.518700</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -12881,7 +12881,7 @@
       </c>
       <c r="Z140" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.519701</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -12971,7 +12971,7 @@
       </c>
       <c r="Z141" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.519701</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -13057,7 +13057,7 @@
       <c r="Y142" t="inlineStr"/>
       <c r="Z142" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.523698</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -13147,7 +13147,7 @@
       </c>
       <c r="Z143" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.524710</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -13233,7 +13233,7 @@
       <c r="Y144" t="inlineStr"/>
       <c r="Z144" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.525699</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -13319,7 +13319,7 @@
       <c r="Y145" t="inlineStr"/>
       <c r="Z145" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.525699</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -13405,7 +13405,7 @@
       <c r="Y146" t="inlineStr"/>
       <c r="Z146" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.526696</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>
@@ -13495,7 +13495,7 @@
       </c>
       <c r="Z147" t="inlineStr">
         <is>
-          <t>2025-11-12T07:25:16.526696</t>
+          <t>2025-11-13T06:53:19.913100</t>
         </is>
       </c>
     </row>

</xml_diff>